<commit_message>
Moved documentation from README into wiki ... Added example for xlsx to valueset conversion ... Added new cds hooks to cds discovery json
</commit_message>
<xml_diff>
--- a/src/test/resources/org/opencds/cqf/test.xlsx
+++ b/src/test/resources/org/opencds/cqf/test.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="413">
   <si>
     <t>2.16.840.1.113883.3.464.1003.103.12.1001</t>
   </si>
@@ -1263,6 +1263,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.6.1</t>
+  </si>
+  <si>
+    <t>cs oid</t>
   </si>
 </sst>
 </file>
@@ -1623,7 +1626,7 @@
   <dimension ref="A1:I239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G243" sqref="G243"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1661,7 +1664,7 @@
         <v>403</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>396</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>